<commit_message>
effects of pandemic programs
</commit_message>
<xml_diff>
--- a/fim archive/fiscal barometer archive/old/FIM BLog Post/forBNPParibas/Hutchins Center Fiscal Barometer 10.2.2014.xlsx
+++ b/fim archive/fiscal barometer archive/old/FIM BLog Post/forBNPParibas/Hutchins Center Fiscal Barometer 10.2.2014.xlsx
@@ -27580,8 +27580,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA9F3DB0CD4D844B918872BCED9B9CF9" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f39872d7210670f8e28df64f3b8e6b7c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cac5d118-ba7b-4807-b700-df6f95cfff50" xmlns:ns3="66951ee6-cd93-49c7-9437-e871b2a117d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b3c5ef4a382acc6fb2d72c08859bf8f" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA9F3DB0CD4D844B918872BCED9B9CF9" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61f75d9b13a46a58fd2456a565edcb9c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cac5d118-ba7b-4807-b700-df6f95cfff50" xmlns:ns3="66951ee6-cd93-49c7-9437-e871b2a117d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d86870d415110e2c98f3a885b29630d1" ns2:_="" ns3:_="">
     <xsd:import namespace="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
     <xsd:import namespace="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
     <xsd:element name="properties">
@@ -27598,6 +27598,10 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -27638,6 +27642,28 @@
     <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="18" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -27786,7 +27812,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69B1152E-6534-4AA3-BD81-9C2B87E5B171}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{433BEC0B-F03C-4239-9D6C-04CD6228817A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>